<commit_message>
close of being done
</commit_message>
<xml_diff>
--- a/Hamming code demenstration.xlsx
+++ b/Hamming code demenstration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10054\OneDrive\ELEC433-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1D8457-419E-456F-A010-F55374877B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F82C7-6660-4ED1-BE31-8FC2C08A04EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,31 +510,31 @@
       </c>
       <c r="N2" s="1">
         <f ca="1">MOD(MOD(SUM(N3:N10,P2:P10,R2:R10,T2:T10),2),2)</f>
-        <v>1.3974885027192308</v>
+        <v>1.4615190960939657</v>
       </c>
       <c r="O2" s="1">
         <f ca="1">MOD(MOD(SUM(O3:P10,S2:T10,P2),2),2)</f>
-        <v>0.68888241232322045</v>
+        <v>3.8411950238870674E-2</v>
       </c>
       <c r="P2">
         <f t="shared" ref="O2:T3" ca="1" si="0">(MOD(RAND(),2))</f>
-        <v>0.46443310633181867</v>
+        <v>0.98506251417930146</v>
       </c>
       <c r="Q2" s="1">
-        <f ca="1">MOD(SUM(Q2:T10),2)</f>
-        <v>0</v>
+        <f ca="1">MOD(SUM(R2:T10,Q3:Q10),2)</f>
+        <v>1.1994973461114427</v>
       </c>
       <c r="R2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18016415585255585</v>
+        <v>0.63813332496253528</v>
       </c>
       <c r="S2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90681925187967949</v>
+        <v>0.52365155735200519</v>
       </c>
       <c r="T2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95335012220506476</v>
+        <v>0.90855274765922955</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -569,36 +569,36 @@
         <v>1</v>
       </c>
       <c r="M3" s="1">
-        <f ca="1">MOD(SUM(M3:T3,M5:T5,M7:T7,M9:T9),2)</f>
-        <v>0</v>
+        <f ca="1">MOD(SUM(N3:T3,M5:T5,M7:T7,M9:T9),2)</f>
+        <v>1.8226099009512495</v>
       </c>
       <c r="N3">
         <f ca="1">(MOD(RAND(),2))</f>
-        <v>0.18685184837274948</v>
+        <v>0.44311169077449319</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35240410002945166</v>
+        <v>0.4028139863431569</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31628164896100464</v>
+        <v>0.58624098897829324</v>
       </c>
       <c r="Q3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30275483686966365</v>
+        <v>0.45180299966245807</v>
       </c>
       <c r="R3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24169736558991117</v>
+        <v>0.47841231670176076</v>
       </c>
       <c r="S3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83619138839119322</v>
+        <v>0.68095166604410284</v>
       </c>
       <c r="T3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2251077195690423</v>
+        <v>2.2183783979021765E-2</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -633,36 +633,36 @@
         <v>2</v>
       </c>
       <c r="M4" s="1">
-        <f ca="1">MOD(SUM(M4:T5,M8:T9),2)</f>
-        <v>0</v>
+        <f ca="1">MOD(SUM(N4:T4,M5:T5,M8:T9),2)</f>
+        <v>0.87858367005804894</v>
       </c>
       <c r="N4">
         <f t="shared" ref="M4:T10" ca="1" si="1">(MOD(RAND(),2))</f>
-        <v>0.3008715344752716</v>
+        <v>0.64881511596853303</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85602874276501406</v>
+        <v>0.56076977921082427</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72309341992661103</v>
+        <v>4.5183724705261663E-2</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36029273840830578</v>
+        <v>0.5707520007320066</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36475529960244324</v>
+        <v>5.9453750369637737E-2</v>
       </c>
       <c r="S4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49517285269313216</v>
+        <v>0.7539490992514607</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39241192981045958</v>
+        <v>0.61397529998100264</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -698,35 +698,35 @@
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6890449095940484</v>
+        <v>0.76621123084687115</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62014712050902532</v>
+        <v>0.28057201705455725</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2269886043403686</v>
+        <v>0.48720773049519683</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25241675328272006</v>
+        <v>0.30623611475924373</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47691445925168474</v>
+        <v>8.194102015975302E-2</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38956402514171518</v>
+        <v>0.53122335419420241</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11000254657843545</v>
+        <v>0.96669033565876838</v>
       </c>
       <c r="T5">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8535001525360304E-2</v>
+        <v>0.73968959567845172</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -761,36 +761,36 @@
         <v>4</v>
       </c>
       <c r="M6" s="1">
-        <f ca="1">MOD(SUM(M6:T9),2)</f>
-        <v>0</v>
+        <f ca="1">MOD(SUM(M7:T9,N6:T6),2)</f>
+        <v>0.46021494406443253</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28358881929479818</v>
+        <v>0.27464085090244539</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21612928444609869</v>
+        <v>0.69391276379534572</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5348193568302998</v>
+        <v>0.27358002867206055</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26348804653069435</v>
+        <v>0.94842845957485944</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79010482531833481</v>
+        <v>0.66002605347242238</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17176394443159759</v>
+        <v>0.21098363306316958</v>
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41876972957274305</v>
+        <v>0.85960898446366207</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -826,35 +826,35 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2911600676373215</v>
+        <v>0.27788250956391203</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69318790634280458</v>
+        <v>0.79697750948528512</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50912209884917037</v>
+        <v>0.9859724574750649</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39518967468442789</v>
+        <v>0.42875372449042737</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89446798840108033</v>
+        <v>0.36970725540133853</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82060355601317325</v>
+        <v>0.91768388540485102</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88907031144141935</v>
+        <v>0.64343501736924291</v>
       </c>
       <c r="T7">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5361701949129833E-2</v>
+        <v>0.65270830993806495</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -890,35 +890,35 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95684214168869242</v>
+        <v>0.17347280410135801</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16351329183392793</v>
+        <v>0.84638144834609907</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18817322665221636</v>
+        <v>0.59264697454637849</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7343825667239342</v>
+        <v>0.2184280114540682</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5058452629509111E-2</v>
+        <v>0.71422500241588682</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52297442636419478</v>
+        <v>0.3251956253363596</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65145183781341964</v>
+        <v>0.91932241922434632</v>
       </c>
       <c r="T8">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9717909215335956E-2</v>
+        <v>0.15204081507504918</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -954,35 +954,35 @@
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26587370367299568</v>
+        <v>0.82622022934431349</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8603455623208429E-2</v>
+        <v>5.2066648057305431E-2</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12051825368496927</v>
+        <v>0.42079565819447007</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97073034574280559</v>
+        <v>0.58589495116176782</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38148785708585187</v>
+        <v>0.28362021049065755</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78513904542389923</v>
+        <v>0.37629545636065009</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52963194757691401</v>
+        <v>0.20233489332676347</v>
       </c>
       <c r="T9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99306984434150847</v>
+        <v>0.77697235355680516</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1022,31 +1022,593 @@
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8082029145252809E-2</v>
+        <v>0.19852675434233935</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10838363344296675</v>
+        <v>0.87890780387086753</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86325244876813811</v>
+        <v>0.78478911799402529</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24680906131300517</v>
+        <v>0.70315723975803357</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24948446098256349</v>
+        <v>0.28822377120090859</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76287505047377269</v>
+        <v>0.46828665185812712</v>
       </c>
       <c r="T10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27723205739300072</v>
+        <v>0.70587845643384561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <v>5</v>
+      </c>
+      <c r="S12">
+        <v>6</v>
+      </c>
+      <c r="T12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <f>MOD(MOD(SUM(C14:C21,E13:E21,G13:G21,I13:I21),2),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f>MOD(MOD(SUM(D14:E21,H13:I21,E13),2),2)</f>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <f>MOD(SUM(G13:I21,F14:F21),2)</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f>MOD(MOD(SUM(N14:N21,P13:P21,R13:R21,T13:T21),2),2)</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <f>MOD(MOD(SUM(O14:P21,S13:T21,P13),2),2)</f>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>MOD(SUM(R13:T21,Q14:Q21),2)</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MOD(SUM(C14:I14,B16:I16,B18:I18,B20:I20),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <f>MOD(SUM(N14:T14,M16:T16,M18:T18,M20:T20),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <f>MOD(SUM(C15:I15,B16:I16,B19:I20),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" s="1">
+        <f>MOD(SUM(N15:T15,M16:T16,M19:T20),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <f>MOD(SUM(B18:I20,C17:I17),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17" s="1">
+        <f>MOD(SUM(M18:T20,N17:T17),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>6</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <f ca="1">MOD(SUM(B21:I21),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21" s="1">
+        <f ca="1">MOD(SUM(M21:T21),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Hamming implementations to slides and reports
</commit_message>
<xml_diff>
--- a/Hamming code demenstration.xlsx
+++ b/Hamming code demenstration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10054\OneDrive\ELEC433-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F82C7-6660-4ED1-BE31-8FC2C08A04EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D51B42-40F5-4C0C-B92E-8CFFF5A5B1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>p0</t>
   </si>
@@ -134,9 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="AQ17" sqref="AQ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,9 +429,11 @@
     <col min="2" max="7" width="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="31" width="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="41" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -479,21 +482,69 @@
       <c r="T1">
         <v>7</v>
       </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Y1">
+        <v>1</v>
+      </c>
+      <c r="Z1">
+        <v>2</v>
+      </c>
+      <c r="AA1">
+        <v>3</v>
+      </c>
+      <c r="AB1">
+        <v>4</v>
+      </c>
+      <c r="AC1">
+        <v>5</v>
+      </c>
+      <c r="AD1">
+        <v>6</v>
+      </c>
+      <c r="AE1">
+        <v>7</v>
+      </c>
+      <c r="AH1">
+        <v>0</v>
+      </c>
+      <c r="AI1">
+        <v>1</v>
+      </c>
+      <c r="AJ1">
+        <v>2</v>
+      </c>
+      <c r="AK1">
+        <v>3</v>
+      </c>
+      <c r="AL1">
+        <v>4</v>
+      </c>
+      <c r="AM1">
+        <v>5</v>
+      </c>
+      <c r="AN1">
+        <v>6</v>
+      </c>
+      <c r="AO1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G2">
@@ -510,38 +561,89 @@
       </c>
       <c r="N2" s="1">
         <f ca="1">MOD(MOD(SUM(N3:N10,P2:P10,R2:R10,T2:T10),2),2)</f>
-        <v>1.4615190960939657</v>
+        <v>0.22676413952444818</v>
       </c>
       <c r="O2" s="1">
         <f ca="1">MOD(MOD(SUM(O3:P10,S2:T10,P2),2),2)</f>
-        <v>3.8411950238870674E-2</v>
+        <v>1.3899130600595182</v>
       </c>
       <c r="P2">
         <f t="shared" ref="O2:T3" ca="1" si="0">(MOD(RAND(),2))</f>
-        <v>0.98506251417930146</v>
+        <v>0.83452450562765701</v>
       </c>
       <c r="Q2" s="1">
         <f ca="1">MOD(SUM(R2:T10,Q3:Q10),2)</f>
-        <v>1.1994973461114427</v>
+        <v>0.34803822071484447</v>
       </c>
       <c r="R2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63813332496253528</v>
+        <v>0.26508364648493776</v>
       </c>
       <c r="S2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52365155735200519</v>
+        <v>0.53644126224995736</v>
       </c>
       <c r="T2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90855274765922955</v>
+        <v>0.46173317266675196</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AE2">
+        <v>3</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK2">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM2">
+        <v>5</v>
+      </c>
+      <c r="AN2">
+        <v>6</v>
+      </c>
+      <c r="AO2">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -570,42 +672,96 @@
       </c>
       <c r="M3" s="1">
         <f ca="1">MOD(SUM(N3:T3,M5:T5,M7:T7,M9:T9),2)</f>
-        <v>1.8226099009512495</v>
+        <v>0.35575963914885556</v>
       </c>
       <c r="N3">
         <f ca="1">(MOD(RAND(),2))</f>
-        <v>0.44311169077449319</v>
+        <v>0.81623480189547604</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4028139863431569</v>
+        <v>0.24166176919399873</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58624098897829324</v>
+        <v>0.70675566681582158</v>
       </c>
       <c r="Q3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45180299966245807</v>
+        <v>0.6365323301078587</v>
       </c>
       <c r="R3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47841231670176076</v>
+        <v>0.49635640393261793</v>
       </c>
       <c r="S3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68095166604410284</v>
+        <v>0.83395798271689503</v>
       </c>
       <c r="T3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2183783979021765E-2</v>
+        <v>0.18599434026583928</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>6</v>
+      </c>
+      <c r="AB3">
+        <v>7</v>
+      </c>
+      <c r="AC3">
+        <v>8</v>
+      </c>
+      <c r="AD3">
+        <v>9</v>
+      </c>
+      <c r="AE3">
+        <v>10</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>8</v>
+      </c>
+      <c r="AI3">
+        <v>9</v>
+      </c>
+      <c r="AJ3">
+        <v>10</v>
+      </c>
+      <c r="AK3">
+        <v>11</v>
+      </c>
+      <c r="AL3">
+        <v>12</v>
+      </c>
+      <c r="AM3">
+        <v>13</v>
+      </c>
+      <c r="AN3">
+        <v>14</v>
+      </c>
+      <c r="AO3">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -634,38 +790,92 @@
       </c>
       <c r="M4" s="1">
         <f ca="1">MOD(SUM(N4:T4,M5:T5,M8:T9),2)</f>
-        <v>0.87858367005804894</v>
+        <v>0.99815405372609867</v>
       </c>
       <c r="N4">
         <f t="shared" ref="M4:T10" ca="1" si="1">(MOD(RAND(),2))</f>
-        <v>0.64881511596853303</v>
+        <v>0.83102987469243284</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56076977921082427</v>
+        <v>0.62763435153296665</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5183724705261663E-2</v>
+        <v>6.8163276836523901E-2</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5707520007320066</v>
+        <v>1.8053919011529196E-4</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9453750369637737E-2</v>
+        <v>0.41531423204158058</v>
       </c>
       <c r="S4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7539490992514607</v>
+        <v>0.62889761120632204</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61397529998100264</v>
+        <v>0.82229568816663068</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4">
+        <v>11</v>
+      </c>
+      <c r="Z4">
+        <v>12</v>
+      </c>
+      <c r="AA4">
+        <v>13</v>
+      </c>
+      <c r="AB4">
+        <v>14</v>
+      </c>
+      <c r="AC4">
+        <v>15</v>
+      </c>
+      <c r="AD4">
+        <v>16</v>
+      </c>
+      <c r="AE4">
+        <v>17</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>16</v>
+      </c>
+      <c r="AI4">
+        <v>17</v>
+      </c>
+      <c r="AJ4">
+        <v>18</v>
+      </c>
+      <c r="AK4">
+        <v>19</v>
+      </c>
+      <c r="AL4">
+        <v>20</v>
+      </c>
+      <c r="AM4">
+        <v>21</v>
+      </c>
+      <c r="AN4">
+        <v>22</v>
+      </c>
+      <c r="AO4">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -698,42 +908,96 @@
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76621123084687115</v>
+        <v>0.76927571201176059</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28057201705455725</v>
+        <v>0.47792848323045378</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48720773049519683</v>
+        <v>3.0259438546190842E-2</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30623611475924373</v>
+        <v>0.17628780303183467</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>8.194102015975302E-2</v>
+        <v>0.17300759189733084</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53122335419420241</v>
+        <v>0.28393349315685767</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96669033565876838</v>
+        <v>0.47673916643105141</v>
       </c>
       <c r="T5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73968959567845172</v>
+        <v>4.2124969134812673E-2</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>18</v>
+      </c>
+      <c r="Y5">
+        <v>19</v>
+      </c>
+      <c r="Z5">
+        <v>20</v>
+      </c>
+      <c r="AA5">
+        <v>20</v>
+      </c>
+      <c r="AB5">
+        <v>20</v>
+      </c>
+      <c r="AC5">
+        <v>20</v>
+      </c>
+      <c r="AD5">
+        <v>20</v>
+      </c>
+      <c r="AE5">
+        <v>25</v>
+      </c>
+      <c r="AG5">
+        <v>3</v>
+      </c>
+      <c r="AH5">
+        <v>24</v>
+      </c>
+      <c r="AI5">
+        <v>25</v>
+      </c>
+      <c r="AJ5">
+        <v>26</v>
+      </c>
+      <c r="AK5">
+        <v>27</v>
+      </c>
+      <c r="AL5">
+        <v>28</v>
+      </c>
+      <c r="AM5">
+        <v>29</v>
+      </c>
+      <c r="AN5">
+        <v>30</v>
+      </c>
+      <c r="AO5">
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6">
@@ -762,38 +1026,92 @@
       </c>
       <c r="M6" s="1">
         <f ca="1">MOD(SUM(M7:T9,N6:T6),2)</f>
-        <v>0.46021494406443253</v>
+        <v>1.5386445575093664</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27464085090244539</v>
+        <v>4.2975130412499229E-2</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69391276379534572</v>
+        <v>0.95156387986643443</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27358002867206055</v>
+        <v>0.66625715395936458</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94842845957485944</v>
+        <v>0.43982679072539088</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66002605347242238</v>
+        <v>5.4508599127011559E-2</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21098363306316958</v>
+        <v>0.10713062111418181</v>
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85960898446366207</v>
+        <v>0.39864432560605045</v>
+      </c>
+      <c r="W6">
+        <v>4</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y6">
+        <v>26</v>
+      </c>
+      <c r="Z6">
+        <v>27</v>
+      </c>
+      <c r="AA6">
+        <v>27</v>
+      </c>
+      <c r="AB6">
+        <v>27</v>
+      </c>
+      <c r="AC6">
+        <v>27</v>
+      </c>
+      <c r="AD6">
+        <v>27</v>
+      </c>
+      <c r="AE6">
+        <v>32</v>
+      </c>
+      <c r="AG6">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>32</v>
+      </c>
+      <c r="AI6">
+        <v>33</v>
+      </c>
+      <c r="AJ6">
+        <v>34</v>
+      </c>
+      <c r="AK6">
+        <v>35</v>
+      </c>
+      <c r="AL6">
+        <v>36</v>
+      </c>
+      <c r="AM6">
+        <v>37</v>
+      </c>
+      <c r="AN6">
+        <v>38</v>
+      </c>
+      <c r="AO6">
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -826,38 +1144,92 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27788250956391203</v>
+        <v>0.96339150068389223</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79697750948528512</v>
+        <v>0.38163801096979932</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9859724574750649</v>
+        <v>0.14382640089264853</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42875372449042737</v>
+        <v>0.69181968920518899</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36970725540133853</v>
+        <v>0.52358260938124057</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91768388540485102</v>
+        <v>0.63279428403896187</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64343501736924291</v>
+        <v>0.15444448552680612</v>
       </c>
       <c r="T7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65270830993806495</v>
+        <v>0.21115925338066377</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>33</v>
+      </c>
+      <c r="Y7">
+        <v>34</v>
+      </c>
+      <c r="Z7">
+        <v>35</v>
+      </c>
+      <c r="AA7">
+        <v>35</v>
+      </c>
+      <c r="AB7">
+        <v>35</v>
+      </c>
+      <c r="AC7">
+        <v>35</v>
+      </c>
+      <c r="AD7">
+        <v>35</v>
+      </c>
+      <c r="AE7">
+        <v>40</v>
+      </c>
+      <c r="AG7">
+        <v>5</v>
+      </c>
+      <c r="AH7">
+        <v>40</v>
+      </c>
+      <c r="AI7">
+        <v>41</v>
+      </c>
+      <c r="AJ7">
+        <v>42</v>
+      </c>
+      <c r="AK7">
+        <v>43</v>
+      </c>
+      <c r="AL7">
+        <v>44</v>
+      </c>
+      <c r="AM7">
+        <v>45</v>
+      </c>
+      <c r="AN7">
+        <v>46</v>
+      </c>
+      <c r="AO7">
+        <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -890,38 +1262,92 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17347280410135801</v>
+        <v>0.30662550203472683</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84638144834609907</v>
+        <v>0.24903443074660181</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59264697454637849</v>
+        <v>0.38448104041098685</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2184280114540682</v>
+        <v>0.81101241520493705</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71422500241588682</v>
+        <v>0.48045814335967774</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3251956253363596</v>
+        <v>0.21768858828612536</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91932241922434632</v>
+        <v>4.8364604624643426E-2</v>
       </c>
       <c r="T8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15204081507504918</v>
+        <v>0.37136364525068266</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>41</v>
+      </c>
+      <c r="Y8">
+        <v>42</v>
+      </c>
+      <c r="Z8">
+        <v>43</v>
+      </c>
+      <c r="AA8">
+        <v>43</v>
+      </c>
+      <c r="AB8">
+        <v>43</v>
+      </c>
+      <c r="AC8">
+        <v>43</v>
+      </c>
+      <c r="AD8">
+        <v>43</v>
+      </c>
+      <c r="AE8">
+        <v>48</v>
+      </c>
+      <c r="AG8">
+        <v>6</v>
+      </c>
+      <c r="AH8">
+        <v>48</v>
+      </c>
+      <c r="AI8">
+        <v>49</v>
+      </c>
+      <c r="AJ8">
+        <v>50</v>
+      </c>
+      <c r="AK8">
+        <v>51</v>
+      </c>
+      <c r="AL8">
+        <v>52</v>
+      </c>
+      <c r="AM8">
+        <v>53</v>
+      </c>
+      <c r="AN8">
+        <v>54</v>
+      </c>
+      <c r="AO8">
+        <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -954,42 +1380,96 @@
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82622022934431349</v>
+        <v>0.41703248847504659</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2066648057305431E-2</v>
+        <v>0.75017765629495226</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42079565819447007</v>
+        <v>0.26303225302716948</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58589495116176782</v>
+        <v>0.29467751675302001</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28362021049065755</v>
+        <v>0.29916974788102124</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37629545636065009</v>
+        <v>0.93073858493062811</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20233489332676347</v>
+        <v>0.82806174711764757</v>
       </c>
       <c r="T9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77697235355680516</v>
+        <v>0.52316345822136656</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9">
+        <v>49</v>
+      </c>
+      <c r="Y9">
+        <v>50</v>
+      </c>
+      <c r="Z9">
+        <v>51</v>
+      </c>
+      <c r="AA9">
+        <v>51</v>
+      </c>
+      <c r="AB9">
+        <v>51</v>
+      </c>
+      <c r="AC9">
+        <v>51</v>
+      </c>
+      <c r="AD9">
+        <v>51</v>
+      </c>
+      <c r="AE9">
+        <v>56</v>
+      </c>
+      <c r="AG9">
+        <v>7</v>
+      </c>
+      <c r="AH9">
+        <v>56</v>
+      </c>
+      <c r="AI9">
+        <v>57</v>
+      </c>
+      <c r="AJ9">
+        <v>58</v>
+      </c>
+      <c r="AK9">
+        <v>59</v>
+      </c>
+      <c r="AL9">
+        <v>60</v>
+      </c>
+      <c r="AM9">
+        <v>61</v>
+      </c>
+      <c r="AN9">
+        <v>62</v>
+      </c>
+      <c r="AO9">
+        <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C10">
@@ -1022,34 +1502,88 @@
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19852675434233935</v>
+        <v>0.69220069445543397</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87890780387086753</v>
+        <v>0.42913702446345292</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78478911799402529</v>
+        <v>0.59131077880041605</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70315723975803357</v>
+        <v>0.27883643109944234</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28822377120090859</v>
+        <v>0.74251810918313599</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46828665185812712</v>
+        <v>0.75767030549321979</v>
       </c>
       <c r="T10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70587845643384561</v>
+        <v>8.9321456717387004E-2</v>
+      </c>
+      <c r="W10">
+        <v>8</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10">
+        <v>57</v>
+      </c>
+      <c r="Z10">
+        <v>58</v>
+      </c>
+      <c r="AA10">
+        <v>58</v>
+      </c>
+      <c r="AB10">
+        <v>58</v>
+      </c>
+      <c r="AC10">
+        <v>58</v>
+      </c>
+      <c r="AD10">
+        <v>58</v>
+      </c>
+      <c r="AE10">
+        <v>63</v>
+      </c>
+      <c r="AG10">
+        <v>8</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>64</v>
+      </c>
+      <c r="AI10">
+        <v>65</v>
+      </c>
+      <c r="AJ10">
+        <v>66</v>
+      </c>
+      <c r="AK10">
+        <v>67</v>
+      </c>
+      <c r="AL10">
+        <v>68</v>
+      </c>
+      <c r="AM10">
+        <v>69</v>
+      </c>
+      <c r="AN10">
+        <v>70</v>
+      </c>
+      <c r="AO10">
+        <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
@@ -1099,7 +1633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1155,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1213,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1271,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>

</xml_diff>